<commit_message>
progress with optimisation procedure
</commit_message>
<xml_diff>
--- a/Prototypes/SimplifiedOrganArbitrator/OptimiseConfig.xlsx
+++ b/Prototypes/SimplifiedOrganArbitrator/OptimiseConfig.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="171">
   <si>
     <t>FodderBeet.Leaf.Photosynthesis.RUE.FixedValue</t>
   </si>
@@ -37,12 +37,6 @@
     <t>Param</t>
   </si>
   <si>
-    <t>RUE</t>
-  </si>
-  <si>
-    <t>RUE_stress_break</t>
-  </si>
-  <si>
     <t>k</t>
   </si>
   <si>
@@ -52,15 +46,6 @@
     <t>k_stress_break</t>
   </si>
   <si>
-    <t>Area_Largest_leaf</t>
-  </si>
-  <si>
-    <t>Area_break_fullstress</t>
-  </si>
-  <si>
-    <t>Area_break_startstress</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -79,9 +64,6 @@
     <t>The area of the larget leaf (m2)</t>
   </si>
   <si>
-    <t>Area_largest_leafPosition</t>
-  </si>
-  <si>
     <t>the main-stem position of the largest leaf</t>
   </si>
   <si>
@@ -100,39 +82,12 @@
     <t>the main-stem position at which leaf senescence begins</t>
   </si>
   <si>
-    <t>The senescence rate when age related senescence starts</t>
-  </si>
-  <si>
-    <t>Sen_Rate_max_cover</t>
-  </si>
-  <si>
-    <t>Sen_break_cover</t>
-  </si>
-  <si>
-    <t>Sen_Rate_max_age</t>
-  </si>
-  <si>
-    <t>Sen_age_start_age</t>
-  </si>
-  <si>
     <t>The main-stem position at which leaf senesecnce reaches a maimum</t>
   </si>
   <si>
-    <t>LeafNconcMin</t>
-  </si>
-  <si>
     <t>The leaf minimum N concentration (g/g)</t>
   </si>
   <si>
-    <t>StoRoot_Carbon_StructuralQ</t>
-  </si>
-  <si>
-    <t>StoRoot_Carbon_MetabolicQ</t>
-  </si>
-  <si>
-    <t>StoRoot_Carbon_StorageQ</t>
-  </si>
-  <si>
     <t>The storage root carbon structural priority coefficient</t>
   </si>
   <si>
@@ -142,42 +97,15 @@
     <t>The storage root carbon storage priority coefficient</t>
   </si>
   <si>
-    <t>StoRoot_Nitrogen_StructuralQ</t>
-  </si>
-  <si>
     <t>The storage root Nitrogen structural priority coefficient</t>
   </si>
   <si>
-    <t>StoRoot_Nitrogen_MetabolicQ</t>
-  </si>
-  <si>
     <t>The storage root Nitrogen metabolic priority coefficient</t>
   </si>
   <si>
-    <t>StoRoot_Nitrogen_StorageQ</t>
-  </si>
-  <si>
     <t>The storage root Nitrogen storage priority coefficient</t>
   </si>
   <si>
-    <t>Leaf_Carbon_StructuralQ</t>
-  </si>
-  <si>
-    <t>Leaf_Carbon_MetabolicQ</t>
-  </si>
-  <si>
-    <t>Leaf_Carbon_StorageQ</t>
-  </si>
-  <si>
-    <t>Leaf_Nitrogen_StructuralQ</t>
-  </si>
-  <si>
-    <t>Leaf_Nitrogen_MetabolicQ</t>
-  </si>
-  <si>
-    <t>Leaf_Nitrogen_StorageQ</t>
-  </si>
-  <si>
     <t>The Leaf carbon structural priority coefficient</t>
   </si>
   <si>
@@ -196,66 +124,33 @@
     <t>The Leaf Nitrogen storage priority coefficient</t>
   </si>
   <si>
-    <t>petiole_Carbon_StructuralQ</t>
-  </si>
-  <si>
     <t>The petiole carbon structural priority coefficient</t>
   </si>
   <si>
-    <t>petiole_Carbon_MetabolicQ</t>
-  </si>
-  <si>
     <t>The petiole carbon metabolic priority coefficient</t>
   </si>
   <si>
-    <t>petiole_Carbon_StorageQ</t>
-  </si>
-  <si>
     <t>The petiole carbon storage priority coefficient</t>
   </si>
   <si>
-    <t>petiole_Nitrogen_StructuralQ</t>
-  </si>
-  <si>
     <t>The petiole Nitrogen structural priority coefficient</t>
   </si>
   <si>
-    <t>petiole_Nitrogen_MetabolicQ</t>
-  </si>
-  <si>
     <t>The petiole Nitrogen metabolic priority coefficient</t>
   </si>
   <si>
-    <t>petiole_Nitrogen_StorageQ</t>
-  </si>
-  <si>
     <t>The petiole Nitrogen storage priority coefficient</t>
   </si>
   <si>
-    <t>Nuptake_WStress_break</t>
-  </si>
-  <si>
     <t>The RWC at which N uptake is limited by water stress</t>
   </si>
   <si>
-    <t>Gsmax</t>
-  </si>
-  <si>
-    <t>R50</t>
-  </si>
-  <si>
     <t>The net radiation at which gs is 50% of max</t>
   </si>
   <si>
-    <t>RFV_max</t>
-  </si>
-  <si>
     <t>Maximum Root front velocity (mm/d)</t>
   </si>
   <si>
-    <t>LeafNconcCrit</t>
-  </si>
-  <si>
     <t>The leaf critical N concentration (g/g)</t>
   </si>
   <si>
@@ -268,36 +163,12 @@
     <t>Max_feasible</t>
   </si>
   <si>
-    <t>Sen_age_max_age</t>
-  </si>
-  <si>
-    <t>Sen_age_max_age + 3</t>
-  </si>
-  <si>
     <t>extinction coefficient multiplier if FW = 0</t>
   </si>
   <si>
-    <t>Area_break_fullstress *0.1</t>
-  </si>
-  <si>
-    <t>Sen_age_start_age+1</t>
-  </si>
-  <si>
-    <t>Sen_age_start_age+45</t>
-  </si>
-  <si>
-    <t>Area_break_fullstress *0.7</t>
-  </si>
-  <si>
     <t>the maximum stomatal conductance at 350 ppm CO2</t>
   </si>
   <si>
-    <t>LeafNconcMin+0.005</t>
-  </si>
-  <si>
-    <t>Nuptake and Response</t>
-  </si>
-  <si>
     <t>LincolnRS2016IrrFullNit0</t>
   </si>
   <si>
@@ -385,18 +256,9 @@
     <t>FodderBeet.StorageRoot.Live.NConc</t>
   </si>
   <si>
-    <t>Potential Canopy</t>
-  </si>
-  <si>
     <t>Potential biomass</t>
   </si>
   <si>
-    <t>Water uptake and response</t>
-  </si>
-  <si>
-    <t>SLA_stress_factor</t>
-  </si>
-  <si>
     <t>The sensitivity of SLA to accumulated water stress in the last 30 days</t>
   </si>
   <si>
@@ -472,9 +334,6 @@
     <t>FodderBeet.Leaf.DeltaLAI.Vegetative.Delta.FW.XYPairs.X[2]</t>
   </si>
   <si>
-    <t>FodderBeet.Root.Network.RootFrontVelocity.PhaseLookupValue.Constant.FixedValue</t>
-  </si>
-  <si>
     <t>FodderBeet.Root.Network.NUptakeSWFactor.XYPairs.X[2]</t>
   </si>
   <si>
@@ -515,6 +374,171 @@
   </si>
   <si>
     <t>FodderBeet.Petiole.Nitrogen.DemandFunctions.QStoragePriority.FixedValue</t>
+  </si>
+  <si>
+    <t>Potential canopy</t>
+  </si>
+  <si>
+    <t>Water response</t>
+  </si>
+  <si>
+    <t>Nitrogen response</t>
+  </si>
+  <si>
+    <t>area_largest_leaf</t>
+  </si>
+  <si>
+    <t>largest_leaf_position</t>
+  </si>
+  <si>
+    <t>cover_sen_rate_max</t>
+  </si>
+  <si>
+    <t>cover_sen_start</t>
+  </si>
+  <si>
+    <t>The senescence rate when age related senescence is at its maximum</t>
+  </si>
+  <si>
+    <t>age_sen_max_rate</t>
+  </si>
+  <si>
+    <t>age_sen_max_node</t>
+  </si>
+  <si>
+    <t>age_sen_start_node</t>
+  </si>
+  <si>
+    <t>rue_stress_break</t>
+  </si>
+  <si>
+    <t>sla_stress_factor</t>
+  </si>
+  <si>
+    <t>area_break_fullstress</t>
+  </si>
+  <si>
+    <t>area_break_startstress</t>
+  </si>
+  <si>
+    <t>rfv_max</t>
+  </si>
+  <si>
+    <t>nuptake_wstress_break</t>
+  </si>
+  <si>
+    <t>gsmax</t>
+  </si>
+  <si>
+    <t>r50</t>
+  </si>
+  <si>
+    <t>leaf_nconc_min</t>
+  </si>
+  <si>
+    <t>leaf_nconc_crit</t>
+  </si>
+  <si>
+    <t>sroot_c_structq</t>
+  </si>
+  <si>
+    <t>sroot_c_metabq</t>
+  </si>
+  <si>
+    <t>sroot_c_storageq</t>
+  </si>
+  <si>
+    <t>leaf_c_structq</t>
+  </si>
+  <si>
+    <t>leaf_c_metabq</t>
+  </si>
+  <si>
+    <t>leaf_c_storageq</t>
+  </si>
+  <si>
+    <t>petiole_c_structq</t>
+  </si>
+  <si>
+    <t>petiole_c_metabq</t>
+  </si>
+  <si>
+    <t>petiole_c_storageq</t>
+  </si>
+  <si>
+    <t>sroot_n_structq</t>
+  </si>
+  <si>
+    <t>sroot_n_metabq</t>
+  </si>
+  <si>
+    <t>sroot_n_storageq</t>
+  </si>
+  <si>
+    <t>leaf_n_structq</t>
+  </si>
+  <si>
+    <t>leaf_n_metabq</t>
+  </si>
+  <si>
+    <t>leaf_n_storageq</t>
+  </si>
+  <si>
+    <t>petiole_n_structq</t>
+  </si>
+  <si>
+    <t>petiole_n_metabq</t>
+  </si>
+  <si>
+    <t>petiole_n_storageq</t>
+  </si>
+  <si>
+    <t>age_sen_start_node + 1</t>
+  </si>
+  <si>
+    <t>age_sen_start_node + 45</t>
+  </si>
+  <si>
+    <t>leaf_nconc_min + 0.005</t>
+  </si>
+  <si>
+    <t>FodderBeet.Root.Network.RootFrontVelocity.PhaseLookupValue.MultiplyFunction.RFVmax</t>
+  </si>
+  <si>
+    <t>rue</t>
+  </si>
+  <si>
+    <t>age_sen_start_node + 24</t>
+  </si>
+  <si>
+    <t>FodderBeet.AboveGroundDead.Wt</t>
+  </si>
+  <si>
+    <t>FodderBeet.AboveGroundDead.N</t>
+  </si>
+  <si>
+    <t>rue_lower_temp_opt</t>
+  </si>
+  <si>
+    <t>Lower temperature optima for RUE</t>
+  </si>
+  <si>
+    <t>fn_rue_break</t>
+  </si>
+  <si>
+    <t>The FNmetabolic value that FN for RUE starts to decrease</t>
+  </si>
+  <si>
+    <t>FodderBeet.Leaf.Photosynthesis.FN.XYPairs.X[2]</t>
+  </si>
+  <si>
+    <t>FodderBeet.Leaf.Photosynthesis.FT.XYPairs.X[2]</t>
+  </si>
+  <si>
+    <t>area_break_startstress * 0.7</t>
+  </si>
+  <si>
+    <t>area_break_startstress * 0.01</t>
   </si>
 </sst>
 </file>
@@ -530,12 +554,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -550,9 +580,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -833,19 +864,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="98" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="84.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="78.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.28515625" customWidth="1"/>
+    <col min="3" max="3" width="37.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
@@ -855,51 +886,51 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H1" t="s">
         <v>78</v>
       </c>
-      <c r="F1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G1" t="s">
-        <v>119</v>
-      </c>
-      <c r="H1" t="s">
-        <v>124</v>
-      </c>
       <c r="I1" t="s">
-        <v>120</v>
+        <v>76</v>
       </c>
       <c r="J1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K1" t="s">
-        <v>89</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
       <c r="D2">
-        <v>3</v>
+        <v>1.7</v>
       </c>
       <c r="E2">
         <v>1.6</v>
@@ -907,77 +938,74 @@
       <c r="F2">
         <v>2.4</v>
       </c>
-      <c r="I2">
+      <c r="H2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>163</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>164</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>168</v>
       </c>
       <c r="D3">
-        <v>0.8</v>
+        <v>22</v>
       </c>
       <c r="E3">
-        <v>0.5</v>
+        <v>10</v>
       </c>
       <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
+        <v>26</v>
+      </c>
+      <c r="H3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="D4">
-        <v>7.4999999999999997E-2</v>
+        <v>0.53</v>
       </c>
       <c r="E4">
-        <v>0.05</v>
+        <v>0.5</v>
       </c>
       <c r="F4">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="I4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>81</v>
       </c>
       <c r="D5">
-        <v>50</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="E5">
-        <v>20</v>
+        <v>0.05</v>
       </c>
       <c r="F5">
-        <v>100</v>
+        <v>0.1</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -985,22 +1013,22 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>82</v>
       </c>
       <c r="D6">
-        <v>5.0000000000000001E-3</v>
+        <v>39</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F6">
-        <v>2.5000000000000001E-2</v>
+        <v>100</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -1008,22 +1036,22 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>83</v>
       </c>
       <c r="D7">
-        <v>0.7</v>
+        <v>1.5E-3</v>
       </c>
       <c r="E7">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>0.9</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -1031,22 +1059,22 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="D8">
-        <v>7.0000000000000001E-3</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F8">
-        <v>0.03</v>
+        <v>0.9</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -1054,22 +1082,22 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>123</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>85</v>
       </c>
       <c r="D9">
-        <v>30</v>
+        <v>1.8E-3</v>
       </c>
       <c r="E9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>50</v>
+        <v>0.03</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -1077,22 +1105,22 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B10" t="s">
-        <v>80</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" t="s">
-        <v>81</v>
-      </c>
-      <c r="E10" t="s">
-        <v>84</v>
-      </c>
-      <c r="F10" t="s">
-        <v>85</v>
+        <v>86</v>
+      </c>
+      <c r="D10">
+        <v>11</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>50</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -1100,76 +1128,82 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>100</v>
-      </c>
-      <c r="I11">
+        <v>87</v>
+      </c>
+      <c r="D11" t="s">
+        <v>160</v>
+      </c>
+      <c r="E11" t="s">
+        <v>155</v>
+      </c>
+      <c r="F11" t="s">
+        <v>156</v>
+      </c>
+      <c r="G11">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" t="s">
-        <v>32</v>
+        <v>88</v>
+      </c>
+      <c r="D12">
+        <v>100</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>100</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>100</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
+        <v>89</v>
+      </c>
+      <c r="D13" t="s">
+        <v>137</v>
+      </c>
+      <c r="E13" t="s">
+        <v>137</v>
+      </c>
+      <c r="F13" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="D14">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1183,53 +1217,59 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" t="s">
-        <v>44</v>
+        <v>91</v>
+      </c>
+      <c r="D15">
+        <v>47</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>100</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16">
-        <v>100</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>100</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
+        <v>92</v>
+      </c>
+      <c r="D16" t="s">
+        <v>140</v>
+      </c>
+      <c r="E16" t="s">
+        <v>140</v>
+      </c>
+      <c r="F16" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>93</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -1243,142 +1283,148 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="C18" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" t="s">
-        <v>56</v>
+        <v>94</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>100</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>100</v>
-      </c>
-      <c r="I19">
-        <v>1</v>
+        <v>95</v>
+      </c>
+      <c r="D19" t="s">
+        <v>143</v>
+      </c>
+      <c r="E19" t="s">
+        <v>143</v>
+      </c>
+      <c r="F19" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="J20">
+        <v>100</v>
+      </c>
+      <c r="I20">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B21" t="s">
-        <v>122</v>
+        <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="F21">
         <v>1</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>77</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F22">
         <v>1</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>145</v>
+        <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>14</v>
+        <v>98</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F23">
         <v>1</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>146</v>
+        <v>5</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -1389,120 +1435,120 @@
       <c r="F24">
         <v>1</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>20</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
+        <v>100</v>
+      </c>
+      <c r="D25" t="s">
+        <v>170</v>
       </c>
       <c r="E25" t="s">
-        <v>83</v>
+        <v>170</v>
       </c>
       <c r="F25" t="s">
-        <v>86</v>
-      </c>
-      <c r="J25">
+        <v>169</v>
+      </c>
+      <c r="J25" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
       <c r="C26" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="D26">
-        <v>100</v>
+        <v>0.01</v>
       </c>
       <c r="E26">
-        <v>5</v>
+        <v>0.3</v>
       </c>
       <c r="F26">
-        <v>100</v>
-      </c>
-      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="J26" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="B27" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>69</v>
+        <v>158</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F27">
-        <v>0.7</v>
-      </c>
-      <c r="J27">
+        <v>100</v>
+      </c>
+      <c r="J27" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="B28" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="C28" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="D28">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="E28">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="F28">
-        <v>0.03</v>
-      </c>
-      <c r="H28">
+        <v>0.7</v>
+      </c>
+      <c r="J28" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
+        <v>103</v>
       </c>
       <c r="D29">
-        <v>50</v>
+        <v>7.7000000000000002E-3</v>
       </c>
       <c r="E29">
-        <v>50</v>
+        <v>1E-3</v>
       </c>
       <c r="F29">
-        <v>200</v>
+        <v>0.03</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -1510,45 +1556,45 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C30" t="s">
-        <v>31</v>
+        <v>104</v>
       </c>
       <c r="D30">
-        <v>2.5000000000000001E-2</v>
+        <v>79</v>
       </c>
       <c r="E30">
-        <v>0.01</v>
+        <v>50</v>
       </c>
       <c r="F30">
-        <v>0.03</v>
-      </c>
-      <c r="K30">
+        <v>200</v>
+      </c>
+      <c r="H30">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="B31" t="s">
-        <v>75</v>
+        <v>166</v>
       </c>
       <c r="C31" t="s">
-        <v>76</v>
+        <v>167</v>
       </c>
       <c r="D31">
-        <v>0.03</v>
-      </c>
-      <c r="E31" t="s">
-        <v>88</v>
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
       </c>
       <c r="F31">
-        <v>3.5000000000000003E-2</v>
+        <v>1</v>
       </c>
       <c r="K31">
         <v>1</v>
@@ -1556,22 +1602,22 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="C32" t="s">
-        <v>39</v>
+        <v>105</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="F32">
-        <v>100</v>
+        <v>0.03</v>
       </c>
       <c r="K32">
         <v>1</v>
@@ -1579,27 +1625,36 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C33" t="s">
-        <v>41</v>
-      </c>
-      <c r="D33" t="s">
-        <v>38</v>
+        <v>106</v>
+      </c>
+      <c r="D33">
+        <v>0.03</v>
+      </c>
+      <c r="E33" t="s">
+        <v>157</v>
+      </c>
+      <c r="F33">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C34" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="D34">
         <v>1</v>
@@ -1616,50 +1671,50 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="B35" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="C35" t="s">
-        <v>53</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35">
-        <v>100</v>
-      </c>
-      <c r="K35">
-        <v>1</v>
+        <v>108</v>
+      </c>
+      <c r="D35" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="B36" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="C36" t="s">
-        <v>54</v>
-      </c>
-      <c r="D36" t="s">
-        <v>47</v>
+        <v>109</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>100</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="B37" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="C37" t="s">
-        <v>55</v>
+        <v>110</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -1676,50 +1731,50 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="B38" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="C38" t="s">
-        <v>63</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38">
-        <v>0</v>
-      </c>
-      <c r="F38">
-        <v>100</v>
-      </c>
-      <c r="K38">
-        <v>1</v>
+        <v>111</v>
+      </c>
+      <c r="D38" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="B39" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="C39" t="s">
-        <v>65</v>
-      </c>
-      <c r="D39" t="s">
-        <v>62</v>
+        <v>112</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>100</v>
+      </c>
+      <c r="K39">
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="B40" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="C40" t="s">
-        <v>67</v>
+        <v>113</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -1730,9 +1785,44 @@
       <c r="F40">
         <v>100</v>
       </c>
+      <c r="K40">
+        <v>1</v>
+      </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K41">
+      <c r="A41" t="s">
+        <v>153</v>
+      </c>
+      <c r="B41" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" t="s">
+        <v>114</v>
+      </c>
+      <c r="D41" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>154</v>
+      </c>
+      <c r="B42" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" t="s">
+        <v>115</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>100</v>
+      </c>
+      <c r="K42">
         <v>1</v>
       </c>
     </row>
@@ -1743,72 +1833,76 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView zoomScale="123" workbookViewId="0">
-      <selection sqref="A1:D1"/>
-    </sheetView>
+    <sheetView zoomScale="123" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B1" t="s">
-        <v>120</v>
+        <v>78</v>
       </c>
       <c r="C1" t="s">
-        <v>121</v>
+        <v>76</v>
       </c>
       <c r="D1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="E1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>93</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
-        <v>95</v>
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1818,41 +1912,45 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E2" sqref="E2:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>96</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C1" t="s">
-        <v>120</v>
+        <v>78</v>
       </c>
       <c r="D1" t="s">
-        <v>121</v>
+        <v>76</v>
       </c>
       <c r="E1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="F1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1863,29 +1961,32 @@
       <c r="E2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>161</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C4">
+        <v>56</v>
+      </c>
+      <c r="B4">
         <v>1</v>
       </c>
       <c r="D4">
@@ -1894,13 +1995,13 @@
       <c r="E4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1908,10 +2009,13 @@
       <c r="E5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>102</v>
+        <v>58</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1919,168 +2023,196 @@
       <c r="E6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>103</v>
+        <v>59</v>
       </c>
       <c r="E7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>162</v>
       </c>
       <c r="E8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>105</v>
-      </c>
-      <c r="E9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>106</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>107</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>108</v>
+        <v>63</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>109</v>
+        <v>64</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>110</v>
+        <v>65</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>111</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>112</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>113</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>114</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>115</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>97</v>
-      </c>
-      <c r="D23">
-        <v>3</v>
+        <v>71</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
progressing optimisation set up
</commit_message>
<xml_diff>
--- a/Prototypes/SimplifiedOrganArbitrator/OptimiseConfig.xlsx
+++ b/Prototypes/SimplifiedOrganArbitrator/OptimiseConfig.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11685"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16410" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="ParamRanges" sheetId="1" r:id="rId1"/>
@@ -867,7 +867,7 @@
   <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,7 +953,7 @@
         <v>168</v>
       </c>
       <c r="D3">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E3">
         <v>10</v>

</xml_diff>

<commit_message>
Tidy up optimize script and params
</commit_message>
<xml_diff>
--- a/Prototypes/SimplifiedOrganArbitrator/OptimiseConfig.xlsx
+++ b/Prototypes/SimplifiedOrganArbitrator/OptimiseConfig.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="168">
   <si>
     <t>FodderBeet.Leaf.Photosynthesis.RUE.FixedValue</t>
   </si>
@@ -337,9 +337,6 @@
     <t>FodderBeet.Leaf.Nitrogen.ConcFunctions.Minimum.FixedValue</t>
   </si>
   <si>
-    <t>FodderBeet.Leaf.Nitrogen.ConcFunctions.Critical.FixedValue</t>
-  </si>
-  <si>
     <t>FodderBeet.StorageRoot.Nitrogen.DemandFunctions.QStructuralPriority.FixedValue</t>
   </si>
   <si>
@@ -490,9 +487,6 @@
     <t>age_sen_start_node + 45</t>
   </si>
   <si>
-    <t>leaf_nconc_min + 0.005</t>
-  </si>
-  <si>
     <t>FodderBeet.Root.Network.RootFrontVelocity.PhaseLookupValue.MultiplyFunction.RFVmax</t>
   </si>
   <si>
@@ -533,6 +527,9 @@
   </si>
   <si>
     <t>BestValue</t>
+  </si>
+  <si>
+    <t>FodderBeet.Leaf.Nitrogen.ConcFunctions.Critical.CritNConc.CritNFactor.FixedValue</t>
   </si>
 </sst>
 </file>
@@ -903,10 +900,10 @@
   <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomRight" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -937,22 +934,22 @@
         <v>43</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G1" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="H1" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>114</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -975,12 +972,12 @@
         <v>0.63</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -998,12 +995,12 @@
         <v>0.05</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -1021,12 +1018,12 @@
         <v>20</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
@@ -1044,12 +1041,12 @@
         <v>1.1999999999999999E-3</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
@@ -1067,15 +1064,15 @@
         <v>0.9</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C7" t="s">
         <v>82</v>
@@ -1090,12 +1087,12 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
@@ -1113,12 +1110,12 @@
         <v>17</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>18</v>
@@ -1127,21 +1124,21 @@
         <v>84</v>
       </c>
       <c r="D9" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>152</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>153</v>
       </c>
       <c r="F9" s="6">
         <v>54</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -1156,24 +1153,24 @@
         <v>2.4</v>
       </c>
       <c r="F10" s="4">
-        <v>1.62</v>
+        <v>1.76</v>
       </c>
       <c r="G10">
         <v>3</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C11" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -1182,18 +1179,18 @@
         <v>26</v>
       </c>
       <c r="F11" s="4">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="G11">
         <v>15</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B12" t="s">
         <v>45</v>
@@ -1214,12 +1211,12 @@
         <v>1E-3</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>39</v>
@@ -1234,18 +1231,18 @@
         <v>200</v>
       </c>
       <c r="F13" s="6">
-        <v>192</v>
+        <v>89.5</v>
       </c>
       <c r="G13" s="5">
         <v>100</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B14" t="s">
         <v>20</v>
@@ -1260,7 +1257,7 @@
         <v>100</v>
       </c>
       <c r="F14" s="4">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -1269,12 +1266,12 @@
         <v>1</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B15" t="s">
         <v>21</v>
@@ -1283,13 +1280,13 @@
         <v>86</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B16" t="s">
         <v>22</v>
@@ -1304,7 +1301,7 @@
         <v>100</v>
       </c>
       <c r="F16" s="4">
-        <v>7</v>
+        <v>11.5</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -1313,12 +1310,12 @@
         <v>1</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B17" t="s">
         <v>26</v>
@@ -1333,7 +1330,7 @@
         <v>100</v>
       </c>
       <c r="F17" s="4">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -1342,12 +1339,12 @@
         <v>1</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B18" t="s">
         <v>27</v>
@@ -1356,13 +1353,13 @@
         <v>89</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B19" t="s">
         <v>28</v>
@@ -1377,7 +1374,7 @@
         <v>100</v>
       </c>
       <c r="F19" s="4">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -1386,12 +1383,12 @@
         <v>1</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B20" t="s">
         <v>32</v>
@@ -1406,7 +1403,7 @@
         <v>100</v>
       </c>
       <c r="F20" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -1415,12 +1412,12 @@
         <v>1</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B21" t="s">
         <v>33</v>
@@ -1429,13 +1426,13 @@
         <v>92</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I21" s="2"/>
     </row>
     <row r="22" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>34</v>
@@ -1450,7 +1447,7 @@
         <v>100</v>
       </c>
       <c r="F22" s="6">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="G22" s="5">
         <v>1</v>
@@ -1459,12 +1456,12 @@
         <v>1</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
@@ -1491,12 +1488,12 @@
         <v>0</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B24" t="s">
         <v>75</v>
@@ -1523,7 +1520,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1543,7 +1540,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="4">
-        <v>0.5</v>
+        <v>0.48</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -1555,7 +1552,7 @@
         <v>1</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1575,7 +1572,7 @@
         <v>1</v>
       </c>
       <c r="F26" s="4">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="G26">
         <v>0</v>
@@ -1587,12 +1584,12 @@
         <v>0</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B27" t="s">
         <v>14</v>
@@ -1604,11 +1601,11 @@
         <v>0</v>
       </c>
       <c r="E27">
+        <v>0.7</v>
+      </c>
+      <c r="F27" s="4">
         <v>0.5</v>
       </c>
-      <c r="F27" s="4">
-        <v>0</v>
-      </c>
       <c r="G27">
         <v>0</v>
       </c>
@@ -1619,12 +1616,12 @@
         <v>0</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B28" t="s">
         <v>13</v>
@@ -1633,13 +1630,13 @@
         <v>98</v>
       </c>
       <c r="D28">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="E28">
         <v>1</v>
       </c>
       <c r="F28" s="4">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G28">
         <v>0.01</v>
@@ -1651,18 +1648,18 @@
         <v>0.01</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B29" t="s">
         <v>40</v>
       </c>
       <c r="C29" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D29">
         <v>5</v>
@@ -1671,7 +1668,7 @@
         <v>100</v>
       </c>
       <c r="F29" s="4">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="G29">
         <v>100</v>
@@ -1683,12 +1680,12 @@
         <v>100</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>38</v>
@@ -1703,7 +1700,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="6">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G30" s="5">
         <v>0</v>
@@ -1715,19 +1712,19 @@
         <v>0</v>
       </c>
       <c r="J30" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B31" t="s">
+        <v>160</v>
+      </c>
+      <c r="C31" t="s">
         <v>161</v>
       </c>
-      <c r="B31" t="s">
-        <v>162</v>
-      </c>
-      <c r="C31" t="s">
-        <v>163</v>
-      </c>
       <c r="D31">
         <v>0</v>
       </c>
@@ -1750,12 +1747,12 @@
         <v>0</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B32" t="s">
         <v>19</v>
@@ -1785,27 +1782,27 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B33" t="s">
         <v>41</v>
       </c>
       <c r="C33" t="s">
-        <v>103</v>
-      </c>
-      <c r="D33" t="s">
-        <v>154</v>
+        <v>167</v>
+      </c>
+      <c r="D33">
+        <v>1.05</v>
       </c>
       <c r="E33">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>154</v>
+        <v>3.5</v>
+      </c>
+      <c r="F33" s="4">
+        <v>1.2</v>
       </c>
       <c r="G33">
         <v>0.03</v>
@@ -1820,18 +1817,18 @@
         <v>0.03</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B34" t="s">
         <v>23</v>
       </c>
       <c r="C34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -1855,33 +1852,33 @@
         <v>1</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B35" t="s">
         <v>24</v>
       </c>
       <c r="C35" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K35" s="2"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B36" t="s">
         <v>25</v>
       </c>
       <c r="C36" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -1905,18 +1902,18 @@
         <v>1</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B37" t="s">
         <v>29</v>
       </c>
       <c r="C37" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -1940,33 +1937,33 @@
         <v>1</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B38" t="s">
         <v>30</v>
       </c>
       <c r="C38" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K38" s="2"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B39" t="s">
         <v>31</v>
       </c>
       <c r="C39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -1990,18 +1987,18 @@
         <v>1</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B40" t="s">
         <v>35</v>
       </c>
       <c r="C40" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -2025,33 +2022,33 @@
         <v>1</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B41" t="s">
         <v>36</v>
       </c>
       <c r="C41" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K41" s="2"/>
     </row>
     <row r="42" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>37</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D42" s="5">
         <v>0</v>
@@ -2075,7 +2072,7 @@
         <v>1</v>
       </c>
       <c r="K42" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2089,7 +2086,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScale="123" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="D2" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2100,19 +2097,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D1" t="s">
         <v>113</v>
       </c>
-      <c r="B1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>114</v>
-      </c>
-      <c r="E1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2170,7 +2167,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2188,19 +2185,19 @@
         <v>52</v>
       </c>
       <c r="B1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" t="s">
         <v>113</v>
       </c>
-      <c r="C1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>114</v>
-      </c>
-      <c r="F1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2222,7 +2219,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2295,7 +2292,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E8">
         <v>1</v>

</xml_diff>